<commit_message>
Results script for laptop
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Third-Year-Project\Intruder-Aircraft-Detection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7A6B4715-E795-4939-B29E-7C91BF8CC2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB2607F-33FB-49E2-8E35-2052B4D7EE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985"/>
+    <workbookView xWindow="6495" yWindow="2835" windowWidth="28800" windowHeight="16575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Tensorflow Image Classifier</t>
   </si>
@@ -98,11 +98,14 @@
   <si>
     <t>Valid</t>
   </si>
+  <si>
+    <t>Learned Quicker</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -659,23 +662,24 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -686,13 +690,15 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1047,11 +1053,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,23 +1070,25 @@
     <col min="7" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1102,167 +1110,180 @@
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="7">
         <v>1000</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="7">
         <v>30</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="7">
         <v>5</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="K3" s="15"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="11" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="15"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="11" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="15"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="12" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="15"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="11" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="15"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="11" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="15"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="11" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="15"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="11" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="15"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="11" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="F3:F11"/>
     <mergeCell ref="G3:G11"/>
-    <mergeCell ref="A1:J1"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="B3:B11"/>
     <mergeCell ref="C3:C11"/>
     <mergeCell ref="D3:D11"/>
     <mergeCell ref="E3:E11"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="K3:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>